<commit_message>
Add Inflation_contributions_graph_data.XLSX, Waterfall_graph_data.XLSX, and trimmed_graph_data.XLSX
</commit_message>
<xml_diff>
--- a/EA_DIFFERENCE.xlsx
+++ b/EA_DIFFERENCE.xlsx
@@ -400,22 +400,22 @@
         <v>43466</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.03</v>
+        <v>0.11</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.566</v>
+        <v>-0.556</v>
       </c>
       <c r="D2" t="n">
         <v>0.352</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.197</v>
+        <v>-0.357</v>
       </c>
       <c r="F2" t="n">
         <v>-0.12</v>
       </c>
       <c r="G2" t="n">
-        <v>1.4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -423,7 +423,7 @@
         <v>43497</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.029</v>
+        <v>0.111</v>
       </c>
       <c r="C3" t="n">
         <v>-0.603</v>
@@ -432,13 +432,13 @@
         <v>0.289</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.181</v>
+        <v>-0.351</v>
       </c>
       <c r="F3" t="n">
         <v>-0.2</v>
       </c>
       <c r="G3" t="n">
-        <v>1.5</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="4">
@@ -446,7 +446,7 @@
         <v>43525</v>
       </c>
       <c r="B4" t="n">
-        <v>0.211</v>
+        <v>0.341</v>
       </c>
       <c r="C4" t="n">
         <v>-0.486</v>
@@ -455,13 +455,13 @@
         <v>0.276</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.087</v>
+        <v>-0.227</v>
       </c>
       <c r="F4" t="n">
         <v>-0.205</v>
       </c>
       <c r="G4" t="n">
-        <v>1.4</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="5">
@@ -469,7 +469,7 @@
         <v>43556</v>
       </c>
       <c r="B5" t="n">
-        <v>0.256</v>
+        <v>0.406</v>
       </c>
       <c r="C5" t="n">
         <v>-0.512</v>
@@ -478,13 +478,13 @@
         <v>0.272</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.029</v>
+        <v>-0.149</v>
       </c>
       <c r="F5" t="n">
         <v>-0.056</v>
       </c>
       <c r="G5" t="n">
-        <v>1.7</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         <v>43586</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.006</v>
+        <v>0.124</v>
       </c>
       <c r="C6" t="n">
         <v>-0.543</v>
@@ -501,13 +501,13 @@
         <v>0.269</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.011</v>
+        <v>-0.141</v>
       </c>
       <c r="F6" t="n">
         <v>0.044</v>
       </c>
       <c r="G6" t="n">
-        <v>1.2</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="7">
@@ -515,7 +515,7 @@
         <v>43617</v>
       </c>
       <c r="B7" t="n">
-        <v>0.047</v>
+        <v>0.177</v>
       </c>
       <c r="C7" t="n">
         <v>-0.487</v>
@@ -524,13 +524,13 @@
         <v>0.276</v>
       </c>
       <c r="E7" t="n">
-        <v>0.011</v>
+        <v>-0.109</v>
       </c>
       <c r="F7" t="n">
         <v>-0.036</v>
       </c>
       <c r="G7" t="n">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="8">
@@ -538,7 +538,7 @@
         <v>43647</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.136</v>
+        <v>0.004</v>
       </c>
       <c r="C8" t="n">
         <v>-0.553</v>
@@ -547,13 +547,13 @@
         <v>0.281</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.145</v>
+        <v>-0.265</v>
       </c>
       <c r="F8" t="n">
         <v>-0.062</v>
       </c>
       <c r="G8" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="9">
@@ -561,22 +561,22 @@
         <v>43678</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.073</v>
+        <v>0.067</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.532</v>
+        <v>-0.522</v>
       </c>
       <c r="D9" t="n">
         <v>0.253</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.121</v>
+        <v>-0.241</v>
       </c>
       <c r="F9" t="n">
         <v>-0.063</v>
       </c>
       <c r="G9" t="n">
-        <v>1</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="10">
@@ -584,22 +584,22 @@
         <v>43709</v>
       </c>
       <c r="B10" t="n">
-        <v>0.027</v>
+        <v>0.167</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.495</v>
+        <v>-0.485</v>
       </c>
       <c r="D10" t="n">
         <v>0.282</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.086</v>
+        <v>-0.196</v>
       </c>
       <c r="F10" t="n">
         <v>0.02</v>
       </c>
       <c r="G10" t="n">
-        <v>0.8</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="11">
@@ -607,22 +607,22 @@
         <v>43739</v>
       </c>
       <c r="B11" t="n">
-        <v>0.047</v>
+        <v>0.187</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.518</v>
+        <v>-0.508</v>
       </c>
       <c r="D11" t="n">
         <v>0.245</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.141</v>
+        <v>-0.251</v>
       </c>
       <c r="F11" t="n">
         <v>0.182</v>
       </c>
       <c r="G11" t="n">
-        <v>0.7</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="12">
@@ -630,22 +630,22 @@
         <v>43770</v>
       </c>
       <c r="B12" t="n">
-        <v>0.114</v>
+        <v>0.244</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.445</v>
+        <v>-0.435</v>
       </c>
       <c r="D12" t="n">
         <v>0.219</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.196</v>
+        <v>-0.336</v>
       </c>
       <c r="F12" t="n">
         <v>0.187</v>
       </c>
       <c r="G12" t="n">
-        <v>1</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="13">
@@ -653,22 +653,22 @@
         <v>43800</v>
       </c>
       <c r="B13" t="n">
-        <v>0.098</v>
+        <v>0.228</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.424</v>
+        <v>-0.414</v>
       </c>
       <c r="D13" t="n">
         <v>0.214</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.151</v>
+        <v>-0.291</v>
       </c>
       <c r="F13" t="n">
         <v>0.082</v>
       </c>
       <c r="G13" t="n">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="14">
@@ -676,22 +676,22 @@
         <v>43831</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.252</v>
+        <v>-0.112</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.296</v>
+        <v>-0.276</v>
       </c>
       <c r="D14" t="n">
         <v>0.194</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.176</v>
+        <v>-0.336</v>
       </c>
       <c r="F14" t="n">
         <v>0.303</v>
       </c>
       <c r="G14" t="n">
-        <v>1.4</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="15">
@@ -699,22 +699,22 @@
         <v>43862</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.277</v>
+        <v>-0.137</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.387</v>
+        <v>-0.367</v>
       </c>
       <c r="D15" t="n">
         <v>0.201</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.209</v>
+        <v>-0.359</v>
       </c>
       <c r="F15" t="n">
         <v>0.348</v>
       </c>
       <c r="G15" t="n">
-        <v>1.2</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="16">
@@ -722,22 +722,22 @@
         <v>43891</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.161</v>
+        <v>-0.031</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.38</v>
+        <v>-0.36</v>
       </c>
       <c r="D16" t="n">
         <v>0.15</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.36</v>
+        <v>-0.49</v>
       </c>
       <c r="F16" t="n">
         <v>0.451</v>
       </c>
       <c r="G16" t="n">
-        <v>0.7</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="17">
@@ -745,22 +745,22 @@
         <v>43922</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.07</v>
+        <v>0.06</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.521</v>
+        <v>-0.501</v>
       </c>
       <c r="D17" t="n">
         <v>0.019</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.473</v>
+        <v>-0.613</v>
       </c>
       <c r="F17" t="n">
         <v>0.398</v>
       </c>
       <c r="G17" t="n">
-        <v>0.3</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="18">
@@ -768,22 +768,22 @@
         <v>43952</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.161</v>
+        <v>-0.031</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.489</v>
+        <v>-0.479</v>
       </c>
       <c r="D18" t="n">
         <v>-0.05</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.468</v>
+        <v>-0.618</v>
       </c>
       <c r="F18" t="n">
         <v>0.296</v>
       </c>
       <c r="G18" t="n">
-        <v>0.1</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="19">
@@ -791,22 +791,22 @@
         <v>43983</v>
       </c>
       <c r="B19" t="n">
-        <v>0.054</v>
+        <v>0.194</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.55</v>
+        <v>-0.54</v>
       </c>
       <c r="D19" t="n">
         <v>-0.098</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.487</v>
+        <v>-0.657</v>
       </c>
       <c r="F19" t="n">
         <v>0.177</v>
       </c>
       <c r="G19" t="n">
-        <v>0.3</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="20">
@@ -814,22 +814,22 @@
         <v>44013</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.445</v>
+        <v>-0.315</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.46</v>
+        <v>-0.44</v>
       </c>
       <c r="D20" t="n">
         <v>-0.115</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.204</v>
+        <v>-0.354</v>
       </c>
       <c r="F20" t="n">
         <v>0.319</v>
       </c>
       <c r="G20" t="n">
-        <v>0.4</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="21">
@@ -837,7 +837,7 @@
         <v>44044</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.397</v>
+        <v>-0.267</v>
       </c>
       <c r="C21" t="n">
         <v>-0.341</v>
@@ -846,13 +846,13 @@
         <v>-0.143</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.237</v>
+        <v>-0.387</v>
       </c>
       <c r="F21" t="n">
         <v>0.266</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.2</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="22">
@@ -860,7 +860,7 @@
         <v>44075</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.103</v>
+        <v>0.017</v>
       </c>
       <c r="C22" t="n">
         <v>-0.42</v>
@@ -869,13 +869,13 @@
         <v>-0.203</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.318</v>
+        <v>-0.458</v>
       </c>
       <c r="F22" t="n">
         <v>0.248</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -883,22 +883,22 @@
         <v>44105</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.32</v>
+        <v>-0.19</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.523</v>
+        <v>-0.513</v>
       </c>
       <c r="D23" t="n">
         <v>-0.245</v>
       </c>
       <c r="E23" t="n">
-        <v>-0.385</v>
+        <v>-0.515</v>
       </c>
       <c r="F23" t="n">
         <v>0.257</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.3</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="24">
@@ -906,22 +906,22 @@
         <v>44136</v>
       </c>
       <c r="B24" t="n">
-        <v>0.024</v>
+        <v>0.154</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.54</v>
+        <v>-0.53</v>
       </c>
       <c r="D24" t="n">
         <v>-0.246</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.333</v>
+        <v>-0.463</v>
       </c>
       <c r="F24" t="n">
         <v>0.331</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.3</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="25">
@@ -929,22 +929,22 @@
         <v>44166</v>
       </c>
       <c r="B25" t="n">
-        <v>0.428</v>
+        <v>0.558</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.617</v>
+        <v>-0.627</v>
       </c>
       <c r="D25" t="n">
         <v>-0.235</v>
       </c>
       <c r="E25" t="n">
-        <v>-0.281</v>
+        <v>-0.401</v>
       </c>
       <c r="F25" t="n">
         <v>0.006</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.3</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="26">
@@ -952,22 +952,22 @@
         <v>44197</v>
       </c>
       <c r="B26" t="n">
-        <v>0.402</v>
+        <v>0.562</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.703</v>
+        <v>-0.683</v>
       </c>
       <c r="D26" t="n">
         <v>-0.2</v>
       </c>
       <c r="E26" t="n">
-        <v>-0.332</v>
+        <v>-0.482</v>
       </c>
       <c r="F26" t="n">
         <v>-0.225</v>
       </c>
       <c r="G26" t="n">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="27">
@@ -975,22 +975,22 @@
         <v>44228</v>
       </c>
       <c r="B27" t="n">
-        <v>0.149</v>
+        <v>0.309</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.836</v>
+        <v>-0.826</v>
       </c>
       <c r="D27" t="n">
         <v>-0.212</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.262</v>
+        <v>-0.422</v>
       </c>
       <c r="F27" t="n">
         <v>-0.193</v>
       </c>
       <c r="G27" t="n">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="28">
@@ -998,7 +998,7 @@
         <v>44256</v>
       </c>
       <c r="B28" t="n">
-        <v>-0.336</v>
+        <v>-0.176</v>
       </c>
       <c r="C28" t="n">
         <v>-0.475</v>
@@ -1007,13 +1007,13 @@
         <v>-0.125</v>
       </c>
       <c r="E28" t="n">
-        <v>-0.029</v>
+        <v>-0.149</v>
       </c>
       <c r="F28" t="n">
         <v>-0.301</v>
       </c>
       <c r="G28" t="n">
-        <v>1.3</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="29">
@@ -1021,7 +1021,7 @@
         <v>44287</v>
       </c>
       <c r="B29" t="n">
-        <v>-0.127</v>
+        <v>0.053</v>
       </c>
       <c r="C29" t="n">
         <v>-0.251</v>
@@ -1030,13 +1030,13 @@
         <v>0.059</v>
       </c>
       <c r="E29" t="n">
-        <v>0.126</v>
+        <v>-0.014</v>
       </c>
       <c r="F29" t="n">
         <v>-0.304</v>
       </c>
       <c r="G29" t="n">
-        <v>1.6</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="30">
@@ -1044,22 +1044,22 @@
         <v>44317</v>
       </c>
       <c r="B30" t="n">
-        <v>0.184</v>
+        <v>0.344</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.249</v>
+        <v>-0.239</v>
       </c>
       <c r="D30" t="n">
         <v>0.109</v>
       </c>
       <c r="E30" t="n">
-        <v>0.042</v>
+        <v>-0.068</v>
       </c>
       <c r="F30" t="n">
         <v>-0.221</v>
       </c>
       <c r="G30" t="n">
-        <v>2</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="31">
@@ -1067,22 +1067,22 @@
         <v>44348</v>
       </c>
       <c r="B31" t="n">
-        <v>-0.055</v>
+        <v>0.105</v>
       </c>
       <c r="C31" t="n">
-        <v>-0.274</v>
+        <v>-0.254</v>
       </c>
       <c r="D31" t="n">
         <v>0.074</v>
       </c>
       <c r="E31" t="n">
-        <v>0.095</v>
+        <v>-0.005</v>
       </c>
       <c r="F31" t="n">
         <v>-0.206</v>
       </c>
       <c r="G31" t="n">
-        <v>1.9</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="32">
@@ -1090,22 +1090,22 @@
         <v>44378</v>
       </c>
       <c r="B32" t="n">
-        <v>0.498</v>
+        <v>0.668</v>
       </c>
       <c r="C32" t="n">
-        <v>-0.438</v>
+        <v>-0.418</v>
       </c>
       <c r="D32" t="n">
         <v>0.087</v>
       </c>
       <c r="E32" t="n">
-        <v>-0.028</v>
+        <v>-0.158</v>
       </c>
       <c r="F32" t="n">
         <v>-0.28</v>
       </c>
       <c r="G32" t="n">
-        <v>2.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -1113,22 +1113,22 @@
         <v>44409</v>
       </c>
       <c r="B33" t="n">
-        <v>0.642</v>
+        <v>0.802</v>
       </c>
       <c r="C33" t="n">
-        <v>-0.719</v>
+        <v>-0.679</v>
       </c>
       <c r="D33" t="n">
         <v>0.193</v>
       </c>
       <c r="E33" t="n">
-        <v>-0.054</v>
+        <v>-0.184</v>
       </c>
       <c r="F33" t="n">
         <v>-0.139</v>
       </c>
       <c r="G33" t="n">
-        <v>3</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="34">
@@ -1136,22 +1136,22 @@
         <v>44440</v>
       </c>
       <c r="B34" t="n">
-        <v>0.281</v>
+        <v>0.461</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.331</v>
+        <v>-0.291</v>
       </c>
       <c r="D34" t="n">
         <v>0.377</v>
       </c>
       <c r="E34" t="n">
-        <v>0.113</v>
+        <v>-0.027</v>
       </c>
       <c r="F34" t="n">
         <v>-0.151</v>
       </c>
       <c r="G34" t="n">
-        <v>3.4</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="35">
@@ -1159,22 +1159,22 @@
         <v>44470</v>
       </c>
       <c r="B35" t="n">
-        <v>0.717</v>
+        <v>0.897</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.136</v>
+        <v>-0.106</v>
       </c>
       <c r="D35" t="n">
         <v>0.483</v>
       </c>
       <c r="E35" t="n">
-        <v>0.139</v>
+        <v>-0.001</v>
       </c>
       <c r="F35" t="n">
         <v>-0.236</v>
       </c>
       <c r="G35" t="n">
-        <v>4.1</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="36">
@@ -1182,22 +1182,22 @@
         <v>44501</v>
       </c>
       <c r="B36" t="n">
-        <v>0.243</v>
+        <v>0.423</v>
       </c>
       <c r="C36" t="n">
-        <v>-0.08</v>
+        <v>-0.03</v>
       </c>
       <c r="D36" t="n">
         <v>0.537</v>
       </c>
       <c r="E36" t="n">
-        <v>0.032</v>
+        <v>-0.098</v>
       </c>
       <c r="F36" t="n">
         <v>-0.265</v>
       </c>
       <c r="G36" t="n">
-        <v>4.9</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="37">
@@ -1205,22 +1205,22 @@
         <v>44531</v>
       </c>
       <c r="B37" t="n">
-        <v>0.064</v>
+        <v>0.254</v>
       </c>
       <c r="C37" t="n">
-        <v>0.163</v>
+        <v>0.213</v>
       </c>
       <c r="D37" t="n">
         <v>0.574</v>
       </c>
       <c r="E37" t="n">
-        <v>-0.173</v>
+        <v>-0.323</v>
       </c>
       <c r="F37" t="n">
         <v>-0.052</v>
       </c>
       <c r="G37" t="n">
-        <v>5</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="38">
@@ -1228,22 +1228,22 @@
         <v>44562</v>
       </c>
       <c r="B38" t="n">
-        <v>-0.307</v>
+        <v>-0.157</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.117</v>
+        <v>-0.077</v>
       </c>
       <c r="D38" t="n">
         <v>0.567</v>
       </c>
       <c r="E38" t="n">
-        <v>0.239</v>
+        <v>0.089</v>
       </c>
       <c r="F38" t="n">
         <v>-0.464</v>
       </c>
       <c r="G38" t="n">
-        <v>5.1</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="39">
@@ -1251,22 +1251,22 @@
         <v>44593</v>
       </c>
       <c r="B39" t="n">
-        <v>-0.276</v>
+        <v>-0.126</v>
       </c>
       <c r="C39" t="n">
-        <v>-0.017</v>
+        <v>0.043</v>
       </c>
       <c r="D39" t="n">
         <v>0.619</v>
       </c>
       <c r="E39" t="n">
-        <v>0.169</v>
+        <v>0.019</v>
       </c>
       <c r="F39" t="n">
         <v>-0.691</v>
       </c>
       <c r="G39" t="n">
-        <v>5.9</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="40">
@@ -1274,22 +1274,22 @@
         <v>44621</v>
       </c>
       <c r="B40" t="n">
-        <v>0.112</v>
+        <v>0.252</v>
       </c>
       <c r="C40" t="n">
-        <v>-0.342</v>
+        <v>-0.272</v>
       </c>
       <c r="D40" t="n">
         <v>0.615</v>
       </c>
       <c r="E40" t="n">
-        <v>-0.062</v>
+        <v>-0.232</v>
       </c>
       <c r="F40" t="n">
         <v>-0.823</v>
       </c>
       <c r="G40" t="n">
-        <v>7.4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">
@@ -1297,22 +1297,22 @@
         <v>44652</v>
       </c>
       <c r="B41" t="n">
-        <v>0.388</v>
+        <v>0.538</v>
       </c>
       <c r="C41" t="n">
-        <v>-0.291</v>
+        <v>-0.211</v>
       </c>
       <c r="D41" t="n">
         <v>0.612</v>
       </c>
       <c r="E41" t="n">
-        <v>-0.42</v>
+        <v>-0.59</v>
       </c>
       <c r="F41" t="n">
         <v>-0.525</v>
       </c>
       <c r="G41" t="n">
-        <v>7.4</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="42">
@@ -1320,22 +1320,22 @@
         <v>44682</v>
       </c>
       <c r="B42" t="n">
-        <v>0.029</v>
+        <v>0.209</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.231</v>
+        <v>-0.131</v>
       </c>
       <c r="D42" t="n">
         <v>0.718</v>
       </c>
       <c r="E42" t="n">
-        <v>-0.339</v>
+        <v>-0.559</v>
       </c>
       <c r="F42" t="n">
         <v>-0.101</v>
       </c>
       <c r="G42" t="n">
-        <v>8.1</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="43">
@@ -1343,22 +1343,22 @@
         <v>44713</v>
       </c>
       <c r="B43" t="n">
-        <v>0.272</v>
+        <v>0.432</v>
       </c>
       <c r="C43" t="n">
-        <v>-0.157</v>
+        <v>-0.057</v>
       </c>
       <c r="D43" t="n">
         <v>0.822</v>
       </c>
       <c r="E43" t="n">
-        <v>-0.27</v>
+        <v>-0.52</v>
       </c>
       <c r="F43" t="n">
         <v>0.214</v>
       </c>
       <c r="G43" t="n">
-        <v>8.6</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="44">
@@ -1366,22 +1366,22 @@
         <v>44743</v>
       </c>
       <c r="B44" t="n">
-        <v>0.446</v>
+        <v>0.626</v>
       </c>
       <c r="C44" t="n">
-        <v>-0.183</v>
+        <v>-0.063</v>
       </c>
       <c r="D44" t="n">
         <v>0.863</v>
       </c>
       <c r="E44" t="n">
-        <v>-0.344</v>
+        <v>-0.624</v>
       </c>
       <c r="F44" t="n">
         <v>-0.034</v>
       </c>
       <c r="G44" t="n">
-        <v>8.9</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="45">
@@ -1389,22 +1389,22 @@
         <v>44774</v>
       </c>
       <c r="B45" t="n">
-        <v>0.301</v>
+        <v>0.481</v>
       </c>
       <c r="C45" t="n">
-        <v>-0.339</v>
+        <v>-0.199</v>
       </c>
       <c r="D45" t="n">
         <v>0.856</v>
       </c>
       <c r="E45" t="n">
-        <v>-0.35</v>
+        <v>-0.66</v>
       </c>
       <c r="F45" t="n">
         <v>-0.577</v>
       </c>
       <c r="G45" t="n">
-        <v>9.1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46">
@@ -1412,22 +1412,22 @@
         <v>44805</v>
       </c>
       <c r="B46" t="n">
-        <v>-0.163</v>
+        <v>0.017</v>
       </c>
       <c r="C46" t="n">
-        <v>-0.484</v>
+        <v>-0.334</v>
       </c>
       <c r="D46" t="n">
         <v>0.688</v>
       </c>
       <c r="E46" t="n">
-        <v>-0.496</v>
+        <v>-0.816</v>
       </c>
       <c r="F46" t="n">
         <v>-0.951</v>
       </c>
       <c r="G46" t="n">
-        <v>9.9</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="47">
@@ -1435,22 +1435,22 @@
         <v>44835</v>
       </c>
       <c r="B47" t="n">
-        <v>-0.493</v>
+        <v>-0.293</v>
       </c>
       <c r="C47" t="n">
-        <v>-0.639</v>
+        <v>-0.469</v>
       </c>
       <c r="D47" t="n">
         <v>0.649</v>
       </c>
       <c r="E47" t="n">
-        <v>-0.576</v>
+        <v>-0.916</v>
       </c>
       <c r="F47" t="n">
         <v>-0.24</v>
       </c>
       <c r="G47" t="n">
-        <v>10.6</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="48">
@@ -1458,22 +1458,22 @@
         <v>44866</v>
       </c>
       <c r="B48" t="n">
-        <v>-0.523</v>
+        <v>-0.303</v>
       </c>
       <c r="C48" t="n">
-        <v>-0.768</v>
+        <v>-0.588</v>
       </c>
       <c r="D48" t="n">
         <v>0.626</v>
       </c>
       <c r="E48" t="n">
-        <v>-0.56</v>
+        <v>-0.93</v>
       </c>
       <c r="F48" t="n">
         <v>0.044</v>
       </c>
       <c r="G48" t="n">
-        <v>10.1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="49">
@@ -1481,22 +1481,22 @@
         <v>44896</v>
       </c>
       <c r="B49" t="n">
-        <v>-0.616</v>
+        <v>-0.406</v>
       </c>
       <c r="C49" t="n">
-        <v>-0.924</v>
+        <v>-0.724</v>
       </c>
       <c r="D49" t="n">
         <v>0.609</v>
       </c>
       <c r="E49" t="n">
-        <v>-0.393</v>
+        <v>-0.803</v>
       </c>
       <c r="F49" t="n">
         <v>0.266</v>
       </c>
       <c r="G49" t="n">
-        <v>9.2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="50">
@@ -1504,22 +1504,22 @@
         <v>44927</v>
       </c>
       <c r="B50" t="n">
-        <v>-1.086</v>
+        <v>-0.796</v>
       </c>
       <c r="C50" t="n">
-        <v>-0.815</v>
+        <v>-0.595</v>
       </c>
       <c r="D50" t="n">
         <v>0.594</v>
       </c>
       <c r="E50" t="n">
-        <v>-0.761</v>
+        <v>-1.191</v>
       </c>
       <c r="F50" t="n">
         <v>0.818</v>
       </c>
       <c r="G50" t="n">
-        <v>8.6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51">
@@ -1527,22 +1527,22 @@
         <v>44958</v>
       </c>
       <c r="B51" t="n">
-        <v>-0.563</v>
+        <v>-0.273</v>
       </c>
       <c r="C51" t="n">
-        <v>-0.781</v>
+        <v>-0.571</v>
       </c>
       <c r="D51" t="n">
         <v>0.58</v>
       </c>
       <c r="E51" t="n">
-        <v>-0.788</v>
+        <v>-1.238</v>
       </c>
       <c r="F51" t="n">
         <v>1.047</v>
       </c>
       <c r="G51" t="n">
-        <v>8.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52">
@@ -1550,22 +1550,22 @@
         <v>44986</v>
       </c>
       <c r="B52" t="n">
-        <v>-0.323</v>
+        <v>-0.033</v>
       </c>
       <c r="C52" t="n">
-        <v>-0.644</v>
+        <v>-0.434</v>
       </c>
       <c r="D52" t="n">
         <v>0.558</v>
       </c>
       <c r="E52" t="n">
-        <v>-0.777</v>
+        <v>-1.277</v>
       </c>
       <c r="F52" t="n">
         <v>1.253</v>
       </c>
       <c r="G52" t="n">
-        <v>6.9</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="53">
@@ -1573,22 +1573,22 @@
         <v>45017</v>
       </c>
       <c r="B53" t="n">
-        <v>-0.979</v>
+        <v>-0.679</v>
       </c>
       <c r="C53" t="n">
-        <v>-0.777</v>
+        <v>-0.567</v>
       </c>
       <c r="D53" t="n">
         <v>0.479</v>
       </c>
       <c r="E53" t="n">
-        <v>-0.362</v>
+        <v>-0.862</v>
       </c>
       <c r="F53" t="n">
         <v>0.862</v>
       </c>
       <c r="G53" t="n">
-        <v>7</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="54">
@@ -1596,22 +1596,22 @@
         <v>45047</v>
       </c>
       <c r="B54" t="n">
-        <v>-0.384</v>
+        <v>-0.074</v>
       </c>
       <c r="C54" t="n">
-        <v>-0.822</v>
+        <v>-0.612</v>
       </c>
       <c r="D54" t="n">
         <v>0.417</v>
       </c>
       <c r="E54" t="n">
-        <v>-0.294</v>
+        <v>-0.784</v>
       </c>
       <c r="F54" t="n">
         <v>0.326</v>
       </c>
       <c r="G54" t="n">
-        <v>6.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="55">
@@ -1619,22 +1619,22 @@
         <v>45078</v>
       </c>
       <c r="B55" t="n">
-        <v>-0.206</v>
+        <v>0.144</v>
       </c>
       <c r="C55" t="n">
-        <v>-0.758</v>
+        <v>-0.568</v>
       </c>
       <c r="D55" t="n">
         <v>0.399</v>
       </c>
       <c r="E55" t="n">
-        <v>-0.435</v>
+        <v>-0.905</v>
       </c>
       <c r="F55" t="n">
         <v>0.256</v>
       </c>
       <c r="G55" t="n">
-        <v>5.5</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="56">
@@ -1642,22 +1642,22 @@
         <v>45108</v>
       </c>
       <c r="B56" t="n">
-        <v>-0.411</v>
+        <v>-0.061</v>
       </c>
       <c r="C56" t="n">
-        <v>-0.894</v>
+        <v>-0.724</v>
       </c>
       <c r="D56" t="n">
         <v>0.385</v>
       </c>
       <c r="E56" t="n">
-        <v>-0.444</v>
+        <v>-0.914</v>
       </c>
       <c r="F56" t="n">
         <v>0.5</v>
       </c>
       <c r="G56" t="n">
-        <v>5.3</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="57">
@@ -1665,22 +1665,22 @@
         <v>45139</v>
       </c>
       <c r="B57" t="n">
-        <v>-0.598</v>
+        <v>-0.238</v>
       </c>
       <c r="C57" t="n">
-        <v>-0.714</v>
+        <v>-0.554</v>
       </c>
       <c r="D57" t="n">
         <v>0.365</v>
       </c>
       <c r="E57" t="n">
-        <v>-0.352</v>
+        <v>-0.792</v>
       </c>
       <c r="F57" t="n">
         <v>0.884</v>
       </c>
       <c r="G57" t="n">
-        <v>5.2</v>
+        <v>2.3</v>
       </c>
     </row>
     <row r="58">
@@ -1688,22 +1688,22 @@
         <v>45170</v>
       </c>
       <c r="B58" t="n">
-        <v>-0.434</v>
+        <v>-0.084</v>
       </c>
       <c r="C58" t="n">
-        <v>-0.675</v>
+        <v>-0.535</v>
       </c>
       <c r="D58" t="n">
         <v>0.419</v>
       </c>
       <c r="E58" t="n">
-        <v>-0.189</v>
+        <v>-0.619</v>
       </c>
       <c r="F58" t="n">
         <v>1.511</v>
       </c>
       <c r="G58" t="n">
-        <v>4.3</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="59">
@@ -1711,22 +1711,22 @@
         <v>45200</v>
       </c>
       <c r="B59" t="n">
-        <v>-0.073</v>
+        <v>0.267</v>
       </c>
       <c r="C59" t="n">
-        <v>-0.558</v>
+        <v>-0.438</v>
       </c>
       <c r="D59" t="n">
         <v>0.379</v>
       </c>
       <c r="E59" t="n">
-        <v>-0.05</v>
+        <v>-0.44</v>
       </c>
       <c r="F59" t="n">
         <v>0.946</v>
       </c>
       <c r="G59" t="n">
-        <v>2.9</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="60">
@@ -1734,22 +1734,22 @@
         <v>45231</v>
       </c>
       <c r="B60" t="n">
-        <v>-0.066</v>
+        <v>0.254</v>
       </c>
       <c r="C60" t="n">
-        <v>-0.548</v>
+        <v>-0.438</v>
       </c>
       <c r="D60" t="n">
         <v>0.366</v>
       </c>
       <c r="E60" t="n">
-        <v>0.033</v>
+        <v>-0.347</v>
       </c>
       <c r="F60" t="n">
         <v>0.229</v>
       </c>
       <c r="G60" t="n">
-        <v>2.4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61">
@@ -1757,22 +1757,22 @@
         <v>45261</v>
       </c>
       <c r="B61" t="n">
-        <v>0.105</v>
+        <v>0.435</v>
       </c>
       <c r="C61" t="n">
-        <v>-0.337</v>
+        <v>-0.247</v>
       </c>
       <c r="D61" t="n">
         <v>0.379</v>
       </c>
       <c r="E61" t="n">
-        <v>0.024</v>
+        <v>-0.306</v>
       </c>
       <c r="F61" t="n">
         <v>0.006</v>
       </c>
       <c r="G61" t="n">
-        <v>2.9</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="62">
@@ -1780,22 +1780,22 @@
         <v>45292</v>
       </c>
       <c r="B62" t="n">
-        <v>0.181</v>
+        <v>0.541</v>
       </c>
       <c r="C62" t="n">
-        <v>-0.513</v>
+        <v>-0.443</v>
       </c>
       <c r="D62" t="n">
         <v>0.368</v>
       </c>
       <c r="E62" t="n">
-        <v>-0.002</v>
+        <v>-0.352</v>
       </c>
       <c r="F62" t="n">
         <v>-0.132</v>
       </c>
       <c r="G62" t="n">
-        <v>2.8</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="63">
@@ -1803,22 +1803,22 @@
         <v>45323</v>
       </c>
       <c r="B63" t="n">
-        <v>0.023</v>
+        <v>0.373</v>
       </c>
       <c r="C63" t="n">
-        <v>-0.586</v>
+        <v>-0.526</v>
       </c>
       <c r="D63" t="n">
         <v>0.318</v>
       </c>
       <c r="E63" t="n">
-        <v>0.191</v>
+        <v>-0.139</v>
       </c>
       <c r="F63" t="n">
         <v>-0.298</v>
       </c>
       <c r="G63" t="n">
-        <v>2.6</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="64">
@@ -1826,22 +1826,22 @@
         <v>45352</v>
       </c>
       <c r="B64" t="n">
-        <v>0</v>
+        <v>0.36</v>
       </c>
       <c r="C64" t="n">
-        <v>-0.718</v>
+        <v>-0.668</v>
       </c>
       <c r="D64" t="n">
         <v>0.283</v>
       </c>
       <c r="E64" t="n">
-        <v>0.241</v>
+        <v>-0.029</v>
       </c>
       <c r="F64" t="n">
         <v>-0.722</v>
       </c>
       <c r="G64" t="n">
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="65">
@@ -1849,16 +1849,16 @@
         <v>45383</v>
       </c>
       <c r="B65" t="n">
-        <v>-0.193</v>
+        <v>0.177</v>
       </c>
       <c r="C65" t="n">
-        <v>-0.676</v>
+        <v>-0.636</v>
       </c>
       <c r="D65" t="n">
         <v>0.276</v>
       </c>
       <c r="E65" t="n">
-        <v>0.272</v>
+        <v>0.012</v>
       </c>
       <c r="F65" t="n">
         <v>-0.609</v>
@@ -1872,22 +1872,22 @@
         <v>45413</v>
       </c>
       <c r="B66" t="n">
-        <v>-0.162</v>
+        <v>0.208</v>
       </c>
       <c r="C66" t="n">
-        <v>-0.677</v>
+        <v>-0.647</v>
       </c>
       <c r="D66" t="n">
         <v>0.259</v>
       </c>
       <c r="E66" t="n">
-        <v>0.2</v>
+        <v>-0.04</v>
       </c>
       <c r="F66" t="n">
         <v>-0.411</v>
       </c>
       <c r="G66" t="n">
-        <v>2.6</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="67">
@@ -1895,22 +1895,22 @@
         <v>45444</v>
       </c>
       <c r="B67" t="n">
-        <v>-0.405</v>
+        <v>-0.035</v>
       </c>
       <c r="C67" t="n">
-        <v>-0.655</v>
+        <v>-0.625</v>
       </c>
       <c r="D67" t="n">
         <v>0.282</v>
       </c>
       <c r="E67" t="n">
-        <v>0.198</v>
+        <v>-0.042</v>
       </c>
       <c r="F67" t="n">
         <v>-0.594</v>
       </c>
       <c r="G67" t="n">
-        <v>2.5</v>
+        <v>1.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Inflation_contributions_graph_data.XLSX, Waterfall_graph_data.XLSX, trimmed_graph_data.XLSX, MEGA_DATA_DOWNLOAD.xlsx,MONTHLY_DATA_DOWNLOAD_ALL.xlsx,QUARTERLY_DATA_DOWNLOAD_ALL.xlsx, SUMMARY_EXPORT_DATA_DOWNLOAD.xlsx and EXPORT_DATA_DOWNLOAD_ALL.xlsx
</commit_message>
<xml_diff>
--- a/EA_DIFFERENCE.xlsx
+++ b/EA_DIFFERENCE.xlsx
@@ -1957,6 +1957,29 @@
         <v>2.1</v>
       </c>
     </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>45536</v>
+      </c>
+      <c r="B70" t="n">
+        <v>-0.274</v>
+      </c>
+      <c r="C70" t="n">
+        <v>-0.646</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0.177</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-0.109</v>
+      </c>
+      <c r="F70" t="n">
+        <v>-0.906</v>
+      </c>
+      <c r="G70" t="n">
+        <v>2.1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Add Inflation_contributions_graph_data.XLSX, Waterfall_graph_data.XLSX, trimmed_graph_data.XLSX, MEGA_DATA_DOWNLOAD.xlsx,VOTEDSPENDING.XLSX,ct.xlsx,tax_revenue.xlsx,MONTHLY_DATA_DOWNLOAD_ALL.xlsx,QUARTERLY_DATA_DOWNLOAD_ALL.xlsx, SUMMARY_EXPORT_DATA_DOWNLOAD.xlsx and EXPORT_DATA_DOWNLOAD_ALL.xlsx
</commit_message>
<xml_diff>
--- a/EA_DIFFERENCE.xlsx
+++ b/EA_DIFFERENCE.xlsx
@@ -2164,6 +2164,52 @@
         <v>79.71</v>
       </c>
     </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>45809</v>
+      </c>
+      <c r="B79" t="n">
+        <v>-0.436</v>
+      </c>
+      <c r="C79" t="n">
+        <v>-0.223</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0.172</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.293</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0.072</v>
+      </c>
+      <c r="G79" t="n">
+        <v>79.67</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>45839</v>
+      </c>
+      <c r="B80" t="n">
+        <v>-0.54</v>
+      </c>
+      <c r="C80" t="n">
+        <v>-0.258</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0.162</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0.272</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0.193</v>
+      </c>
+      <c r="G80" t="n">
+        <v>79.59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>